<commit_message>
cc to email jobs
</commit_message>
<xml_diff>
--- a/reports/_APL BANGLADESH PVT LTD_ISPAHANI SUMMIT ALLIANCE TERMINALS LIMITED_container_report_2018-12-27_2_.xlsx
+++ b/reports/_APL BANGLADESH PVT LTD_ISPAHANI SUMMIT ALLIANCE TERMINALS LIMITED_container_report_2018-12-27_2_.xlsx
@@ -3500,7 +3500,7 @@
         </is>
       </c>
       <c r="P6" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q6" s="0" t="n">
         <v>1</v>
@@ -3766,7 +3766,7 @@
         </is>
       </c>
       <c r="P9" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="0" t="n">
         <v>1</v>

</xml_diff>

<commit_message>
do not send empty reports
</commit_message>
<xml_diff>
--- a/reports/_APL BANGLADESH PVT LTD_ISPAHANI SUMMIT ALLIANCE TERMINALS LIMITED_container_report_2018-12-27_2_.xlsx
+++ b/reports/_APL BANGLADESH PVT LTD_ISPAHANI SUMMIT ALLIANCE TERMINALS LIMITED_container_report_2018-12-27_2_.xlsx
@@ -105,7 +105,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X22"/>
+  <dimension ref="A1:X23"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -131,7 +131,7 @@
     <col min="18" max="18" bestFit="true" customWidth="true" width="10.4561797752809"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="24.8561797752809"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="23.0561797752809"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="36.08988764044944"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="40.489887640449446"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="28.4561797752809"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="21.2561797752809"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="19.4561797752809"/>
@@ -161,7 +161,7 @@
     <row ht="16" customHeight="true" r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Total number of containers : 13</t>
+          <t>Total number of containers : 14</t>
         </is>
       </c>
     </row>
@@ -1780,6 +1780,108 @@
       <c r="V22" s="0"/>
       <c r="W22" s="0"/>
       <c r="X22" s="0"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>845</v>
+      </c>
+      <c r="C23" s="0" t="inlineStr">
+        <is>
+          <t>FCIU8790621</t>
+        </is>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E23" s="0" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="F23" s="0" t="inlineStr">
+        <is>
+          <t>ISATL</t>
+        </is>
+      </c>
+      <c r="G23" s="0" t="inlineStr">
+        <is>
+          <t>ISATL</t>
+        </is>
+      </c>
+      <c r="H23" s="0" t="inlineStr">
+        <is>
+          <t>APL</t>
+        </is>
+      </c>
+      <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>APL</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
+        <is>
+          <t>CPA</t>
+        </is>
+      </c>
+      <c r="K23" s="0" t="inlineStr">
+        <is>
+          <t>TR ARAMIS V 016N</t>
+        </is>
+      </c>
+      <c r="L23" s="0" t="inlineStr">
+        <is>
+          <t>2018/3965</t>
+        </is>
+      </c>
+      <c r="M23" s="4" t="d">
+        <v>2018-12-26T12:44:20</v>
+      </c>
+      <c r="N23" s="0" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="O23" s="0"/>
+      <c r="P23" s="0"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="S23" s="0" t="inlineStr">
+        <is>
+          <t>FLOORS-()</t>
+        </is>
+      </c>
+      <c r="T23" s="0" t="inlineStr">
+        <is>
+          <t>Floor board-()</t>
+        </is>
+      </c>
+      <c r="U23" s="0" t="inlineStr">
+        <is>
+          <t>flooor board dirty by oil stain ,black stain ,&amp; ink dirty </t>
+        </is>
+      </c>
+      <c r="V23" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W23" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="X23" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
@@ -1984,7 +2086,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>2</v>
@@ -1993,10 +2095,10 @@
         <v>0</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3225,7 +3327,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB27"/>
+  <dimension ref="A1:AB28"/>
   <sheetViews>
     <sheetView windowProtection="false" tabSelected="false" showWhiteSpace="false" showOutlineSymbols="false" showFormulas="false" rightToLeft="false" showZeros="true" showRuler="true" showRowColHeaders="true" showGridLines="true" defaultGridColor="true" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -3255,7 +3357,7 @@
     <col min="22" max="22" bestFit="true" customWidth="true" width="10.78988764044944"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="24.8561797752809"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="25.08988764044944"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="36.08988764044944"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="40.489887640449446"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="28.4561797752809"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="21.2561797752809"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="19.4561797752809"/>
@@ -3285,7 +3387,7 @@
     <row ht="16" customHeight="true" r="4">
       <c r="A4" s="3" t="inlineStr">
         <is>
-          <t>Total number of containers : 17</t>
+          <t>Total number of containers : 18</t>
         </is>
       </c>
     </row>
@@ -5570,6 +5672,120 @@
       <c r="Z27" s="0"/>
       <c r="AA27" s="0"/>
       <c r="AB27" s="0"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>845</v>
+      </c>
+      <c r="C28" s="0" t="inlineStr">
+        <is>
+          <t>FCIU8790621</t>
+        </is>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="E28" s="0" t="inlineStr">
+        <is>
+          <t>HC</t>
+        </is>
+      </c>
+      <c r="F28" s="0" t="inlineStr">
+        <is>
+          <t>APL</t>
+        </is>
+      </c>
+      <c r="G28" s="0" t="inlineStr">
+        <is>
+          <t>APL</t>
+        </is>
+      </c>
+      <c r="H28" s="0" t="inlineStr">
+        <is>
+          <t>ISATL</t>
+        </is>
+      </c>
+      <c r="I28" s="0" t="inlineStr">
+        <is>
+          <t>ISATL</t>
+        </is>
+      </c>
+      <c r="J28" s="0" t="inlineStr">
+        <is>
+          <t>TR ARAMIS V 016N</t>
+        </is>
+      </c>
+      <c r="K28" s="0" t="inlineStr">
+        <is>
+          <t>2018/3965</t>
+        </is>
+      </c>
+      <c r="L28" s="0" t="inlineStr">
+        <is>
+          <t>CPA</t>
+        </is>
+      </c>
+      <c r="M28" s="4" t="d">
+        <v>2018-12-26T12:44:20</v>
+      </c>
+      <c r="N28" s="0" t="inlineStr">
+        <is>
+          <t>WASH</t>
+        </is>
+      </c>
+      <c r="O28" s="0"/>
+      <c r="P28" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="R28" s="0" t="inlineStr">
+        <is>
+          <t>Empty</t>
+        </is>
+      </c>
+      <c r="S28" s="0"/>
+      <c r="T28" s="0"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="W28" s="0" t="inlineStr">
+        <is>
+          <t>FLOORS-()</t>
+        </is>
+      </c>
+      <c r="X28" s="0" t="inlineStr">
+        <is>
+          <t>Floor board-()</t>
+        </is>
+      </c>
+      <c r="Y28" s="0" t="inlineStr">
+        <is>
+          <t>flooor board dirty by oil stain ,black stain ,&amp; ink dirty </t>
+        </is>
+      </c>
+      <c r="Z28" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AA28" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
+      <c r="AB28" s="0" t="inlineStr">
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="true"/>
@@ -5774,7 +5990,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I7" s="0" t="n">
         <v>2</v>
@@ -5783,10 +5999,10 @@
         <v>3</v>
       </c>
       <c r="K7" s="0" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="L7" s="0" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>